<commit_message>
Manuál teszt kiegészítése további tesztekkel
</commit_message>
<xml_diff>
--- a/documentation/Tutorialbase_Test_Catalog_Final.xlsx
+++ b/documentation/Tutorialbase_Test_Catalog_Final.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zolee\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\tutorialbase\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06E33845-CA37-43C8-816E-935FF0974956}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D09BAE5-F8A5-4092-9338-D0A99B41A28F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E6931828-F469-4112-9B69-B19824B4D461}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="487">
   <si>
     <t>Teszt azonosító</t>
   </si>
@@ -1092,6 +1092,483 @@
   </si>
   <si>
     <t>Dátum</t>
+  </si>
+  <si>
+    <t>Feltöltés gomb aktiválódik, ha minden mező ki van töltve</t>
+  </si>
+  <si>
+    <t>Tölts ki minden mezőt, válassz kategóriát és tölts fel érvényes képet és videót</t>
+  </si>
+  <si>
+    <t>Feltöltés gomb aktív</t>
+  </si>
+  <si>
+    <t>Feltöltés gomb aktív, kattintható</t>
+  </si>
+  <si>
+    <t>Alkategória mező aktívvá válik kategória kiválasztás után</t>
+  </si>
+  <si>
+    <t>Válassz egy főkategóriát</t>
+  </si>
+  <si>
+    <t>Alkategória mező aktív</t>
+  </si>
+  <si>
+    <t>Alkategória mező aktívvá vált</t>
+  </si>
+  <si>
+    <t>PNG fájl feltöltése képként</t>
+  </si>
+  <si>
+    <t>Tölts fel egy PNG fájlt képként</t>
+  </si>
+  <si>
+    <t>Kép megjelenik az előnézeti mezőben</t>
+  </si>
+  <si>
+    <t>Kép megjelenik</t>
+  </si>
+  <si>
+    <t>MP4 videó feltöltése</t>
+  </si>
+  <si>
+    <t>Tölts fel egy MP4 fájlt</t>
+  </si>
+  <si>
+    <t>Videó elfogadva</t>
+  </si>
+  <si>
+    <t>Cím hossza pontosan 100 karakter</t>
+  </si>
+  <si>
+    <t>Adj meg egy pontosan 100 karakter hosszú címet</t>
+  </si>
+  <si>
+    <t>Nem jelenik meg hiba</t>
+  </si>
+  <si>
+    <t>Nem jelent meg hiba</t>
+  </si>
+  <si>
+    <t>Leírás hossza pontosan 600 karakter</t>
+  </si>
+  <si>
+    <t>Adj meg egy pontosan 600 karakter hosszú leírást</t>
+  </si>
+  <si>
+    <t>Kevesebb mint 5 tag megadása helyes formátumban</t>
+  </si>
+  <si>
+    <t>Írd be: `video1,video2`</t>
+  </si>
+  <si>
+    <t>Nincs hiba, mező elfogadva</t>
+  </si>
+  <si>
+    <t>Nincs hiba</t>
+  </si>
+  <si>
+    <t>Max. 5 tag megadása helyes formátumban</t>
+  </si>
+  <si>
+    <t>Írd be: `tag1,tag2,tag3,tag4,tag5`</t>
+  </si>
+  <si>
+    <t>Mező elfogadva</t>
+  </si>
+  <si>
+    <t>Feltöltés gomb inaktív, ha hiányzik a leírás</t>
+  </si>
+  <si>
+    <t>Ne adj meg leírást, de a többi mezőt töltsd ki</t>
+  </si>
+  <si>
+    <t>Feltöltés gomb inaktív marad</t>
+  </si>
+  <si>
+    <t>Feltöltés gomb nem aktiválódott</t>
+  </si>
+  <si>
+    <t>Hibás formátumú kép visszautasítása</t>
+  </si>
+  <si>
+    <t>Próbálj feltölteni `.bmp` képet</t>
+  </si>
+  <si>
+    <t>Hibaüzenet: „Érvénytelen fájlformátum”</t>
+  </si>
+  <si>
+    <t>Hibaüzenet megjelent</t>
+  </si>
+  <si>
+    <t>Hibás videóformátum visszautasítása</t>
+  </si>
+  <si>
+    <t>Próbálj `.avi` fájlt feltölteni</t>
+  </si>
+  <si>
+    <t>Szóközös tagek visszautasítása</t>
+  </si>
+  <si>
+    <t>Írd be: `tag 1,tag2`</t>
+  </si>
+  <si>
+    <t>Hibaüzenet jelenik meg</t>
+  </si>
+  <si>
+    <t>Hibaüzenet: „Érvénytelen formátum”</t>
+  </si>
+  <si>
+    <t>Dupla vessző hibás tagnál</t>
+  </si>
+  <si>
+    <t>Írd be: `tag1,,tag2`</t>
+  </si>
+  <si>
+    <t>Hibaüzenet: „Érvénytelen tagformátum”</t>
+  </si>
+  <si>
+    <t>Kép megjelenik előnézetben feltöltés után</t>
+  </si>
+  <si>
+    <t>Tölts fel érvényes JPG képet</t>
+  </si>
+  <si>
+    <t>A kép látható az előnézeti dobozban</t>
+  </si>
+  <si>
+    <t>A kép megjelent</t>
+  </si>
+  <si>
+    <t>Alkategória listája a főkategória szerint frissül</t>
+  </si>
+  <si>
+    <t>Válassz főkategóriát, figyeld az alkategória opciók változását</t>
+  </si>
+  <si>
+    <t>Az alkategória lehetőségek az API alapján frissülnek</t>
+  </si>
+  <si>
+    <t>Alkategória opciók megváltoztak kategória szerint</t>
+  </si>
+  <si>
+    <t>TC 71</t>
+  </si>
+  <si>
+    <t>TC 72</t>
+  </si>
+  <si>
+    <t>TC 73</t>
+  </si>
+  <si>
+    <t>TC 74</t>
+  </si>
+  <si>
+    <t>TC 75</t>
+  </si>
+  <si>
+    <t>TC 76</t>
+  </si>
+  <si>
+    <t>TC 77</t>
+  </si>
+  <si>
+    <t>TC 78</t>
+  </si>
+  <si>
+    <t>TC 79</t>
+  </si>
+  <si>
+    <t>TC 80</t>
+  </si>
+  <si>
+    <t>TC 81</t>
+  </si>
+  <si>
+    <t>TC 82</t>
+  </si>
+  <si>
+    <t>TC 83</t>
+  </si>
+  <si>
+    <t>TC 84</t>
+  </si>
+  <si>
+    <t>TC 85</t>
+  </si>
+  <si>
+    <t>Kötelező mezők kitöltése</t>
+  </si>
+  <si>
+    <t>1. Nyisd meg a feltöltési oldalt. 2. Töltsd ki az összes kötelező mezőt helyes adatokat használva. 3. Ellenőrizd, hogy a „Feltöltés” gomb aktív.</t>
+  </si>
+  <si>
+    <t>A gomb aktív és megnyomható.</t>
+  </si>
+  <si>
+    <t>A kötelező mezők kitöltése után a gomb aktívvá vált.</t>
+  </si>
+  <si>
+    <t>Feltöltés indítása</t>
+  </si>
+  <si>
+    <t>1. Kattints a „Feltöltés” gombra. 2. Figyeld meg a progress bar megjelenését a gomb alatt.</t>
+  </si>
+  <si>
+    <t>A progress bar megjelenik és mutatja a feltöltés állapotát.</t>
+  </si>
+  <si>
+    <t>A feltöltési gombra kattintva megjelent a progress bar.</t>
+  </si>
+  <si>
+    <t>Sikeres feltöltés visszajelzése</t>
+  </si>
+  <si>
+    <t>1. Várd meg, hogy a feltöltés befejeződjön. 2. Figyeld meg az alert üzenetet.</t>
+  </si>
+  <si>
+    <t>„Sikeres feltöltés” alert jelenik meg.</t>
+  </si>
+  <si>
+    <t>Feltöltés végén megjelent a sikeres alert üzenet.</t>
+  </si>
+  <si>
+    <t>Sikertelen feltöltés visszajelzése</t>
+  </si>
+  <si>
+    <t>1. Próbálj meg hibás fájlt vagy hiányos adatokat feltölteni. 2. Figyeld meg az alert üzenetet.</t>
+  </si>
+  <si>
+    <t>„Sikertelen feltöltés” alert jelenik meg.</t>
+  </si>
+  <si>
+    <t>Hibás fájl feltöltésekor megjelent a sikertelen alert üzenet.</t>
+  </si>
+  <si>
+    <t>Responsivitás mobil nézetben</t>
+  </si>
+  <si>
+    <t>1. Nyisd meg az oldalt mobil eszközön. 2. Figyeld meg az elrendezést és a gombok működését.</t>
+  </si>
+  <si>
+    <t>Az oldal megfelelően alkalmazkodik a mobil kijelzőhöz.</t>
+  </si>
+  <si>
+    <t>Az oldal mobil nézetben megfelelően jelenik meg, minden elem jól látható és használható.</t>
+  </si>
+  <si>
+    <t>Responsivitás tablet nézetben</t>
+  </si>
+  <si>
+    <t>1. Nyisd meg az oldalt tableten. 2. Ellenőrizd a funkciók működését.</t>
+  </si>
+  <si>
+    <t>Az oldal megfelelően jelenik meg és használható.</t>
+  </si>
+  <si>
+    <t>Az oldal tableten megfelelően alkalmazkodik, minden funkció elérhető.</t>
+  </si>
+  <si>
+    <t>Responsivitás kis méretű ablakban</t>
+  </si>
+  <si>
+    <t>1. Nyisd meg az oldalt asztali böngészőben és csökkentsd az ablak méretét. 2. Ellenőrizd az automatikus átrendeződést.</t>
+  </si>
+  <si>
+    <t>Az oldal sikeresen átalakul, és minden funkció elérhető marad.</t>
+  </si>
+  <si>
+    <t>Az oldal megfelelően reagál a kisebb ablakméretre, az elemek átrendeződnek és használhatók maradnak.</t>
+  </si>
+  <si>
+    <t>UI/UX</t>
+  </si>
+  <si>
+    <t>Feltöltés gombok aktiválása</t>
+  </si>
+  <si>
+    <t>1. Nincs fájl kiválasztva, vagy nincs bio-szöveg beírva. 2. Figyeld meg a feltöltési gombokat.</t>
+  </si>
+  <si>
+    <t>A gombok le vannak tiltva.</t>
+  </si>
+  <si>
+    <t>A gombok inaktívak, amíg nincs fájl vagy bio-szöveg.</t>
+  </si>
+  <si>
+    <t>Bio karakterkorlát tesztelése</t>
+  </si>
+  <si>
+    <t>1. Írj be szöveget a bio mezőbe. 2. Próbáld meg túllépni a maximális karakterkorlátot.</t>
+  </si>
+  <si>
+    <t>Nem enged több karaktert beírni.</t>
+  </si>
+  <si>
+    <t>A rendszer megfelelően korlátozza a karakterek számát.</t>
+  </si>
+  <si>
+    <t>Fiók törlés tesztelése</t>
+  </si>
+  <si>
+    <t>1. Kattints a törlés gombra. 2. Figyeld meg az alert üzenetet. 3. Nyomj „Confirm”-ot.</t>
+  </si>
+  <si>
+    <t>A fiók törlődik és kijelentkeztet.</t>
+  </si>
+  <si>
+    <t>Törlés után a rendszer kijelentkeztetett.</t>
+  </si>
+  <si>
+    <t>Lenyíló menük viselkedése</t>
+  </si>
+  <si>
+    <t>1. Kattints egy kategóriamenüre, majd egy profilmenüre.</t>
+  </si>
+  <si>
+    <t>Az első menü bezárul.</t>
+  </si>
+  <si>
+    <t>Az első menü automatikusan bezáródik.</t>
+  </si>
+  <si>
+    <t>Navbar bejelentkezési állapot</t>
+  </si>
+  <si>
+    <t>1. Figyeld meg a navbar jobb szélét bejelentkezés előtt és után.</t>
+  </si>
+  <si>
+    <t>Bejelentkezés előtt: Bejelentkezés gomb. Bejelentkezés után: Profil ikon.</t>
+  </si>
+  <si>
+    <t>A navbar megfelelően változik a státusz szerint.</t>
+  </si>
+  <si>
+    <t>Komment megjelenése</t>
+  </si>
+  <si>
+    <t>1. Írj egy kommentet. 2. Figyeld meg a helyét az oldalon.</t>
+  </si>
+  <si>
+    <t>A komment a tetején jelenik meg.</t>
+  </si>
+  <si>
+    <t>A komment helyesen a tetején jelenik meg.</t>
+  </si>
+  <si>
+    <t>Nem létező URL megnyitása</t>
+  </si>
+  <si>
+    <t>1. Írj be egy nem létező URL-t. 2. Figyeld meg az oldal viselkedését.</t>
+  </si>
+  <si>
+    <t>Nem jelenik meg semmi az oldalon.</t>
+  </si>
+  <si>
+    <t>Az oldal nem töltött be tartalmat.</t>
+  </si>
+  <si>
+    <t>Videó interakciós teszt</t>
+  </si>
+  <si>
+    <t>1. Kattints a like/dislike gombra.</t>
+  </si>
+  <si>
+    <t>Like = zöld ikon, Dislike = piros ikon.</t>
+  </si>
+  <si>
+    <t>Ikonok megfelelő színnel változnak.</t>
+  </si>
+  <si>
+    <t>Üres keresési eredmények</t>
+  </si>
+  <si>
+    <t>1. Keress rá egy nem létező videóra.</t>
+  </si>
+  <si>
+    <t>„Nincs találat” üzenet jelenik meg.</t>
+  </si>
+  <si>
+    <t>A rendszer megfelelően jelzi, ha nincs találat.</t>
+  </si>
+  <si>
+    <t>Üres előzmények tesztelése</t>
+  </si>
+  <si>
+    <t>1. Nyisd meg a videóelőzmények oldalt, ha nincs előzmény.</t>
+  </si>
+  <si>
+    <t>„Nincs előzmény” üzenet jelenik meg.</t>
+  </si>
+  <si>
+    <t>A rendszer megfelelően jelzi az üres előzményeket.</t>
+  </si>
+  <si>
+    <t>Üres feltöltések tesztelése</t>
+  </si>
+  <si>
+    <t>1. Nyisd meg a felhasználó feltöltéseit, ha nincs videó feltöltve.</t>
+  </si>
+  <si>
+    <t>„Nincs videó” üzenet jelenik meg.</t>
+  </si>
+  <si>
+    <t>A rendszer megfelelően jelzi az üres feltöltéseket.</t>
+  </si>
+  <si>
+    <t>TC 86</t>
+  </si>
+  <si>
+    <t>TC 87</t>
+  </si>
+  <si>
+    <t>TC 88</t>
+  </si>
+  <si>
+    <t>TC 89</t>
+  </si>
+  <si>
+    <t>TC 90</t>
+  </si>
+  <si>
+    <t>TC 91</t>
+  </si>
+  <si>
+    <t>TC 92</t>
+  </si>
+  <si>
+    <t>TC 93</t>
+  </si>
+  <si>
+    <t>TC 94</t>
+  </si>
+  <si>
+    <t>TC 95</t>
+  </si>
+  <si>
+    <t>TC 96</t>
+  </si>
+  <si>
+    <t>TC 97</t>
+  </si>
+  <si>
+    <t>TC 98</t>
+  </si>
+  <si>
+    <t>TC 99</t>
+  </si>
+  <si>
+    <t>TC 100</t>
+  </si>
+  <si>
+    <t>TC 101</t>
+  </si>
+  <si>
+    <t>TC 102</t>
+  </si>
+  <si>
+    <t>TC 103</t>
   </si>
 </sst>
 </file>
@@ -1548,17 +2025,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6912224A-70CB-4078-919C-90B53996CAF2}">
-  <dimension ref="A1:H72"/>
+  <dimension ref="A1:H104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C79" sqref="C79"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I94" sqref="I94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="60.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="127.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="97.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="58.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="53.7109375" style="1" bestFit="1" customWidth="1"/>
@@ -1642,7 +2119,7 @@
         <v>7</v>
       </c>
       <c r="H3" s="8">
-        <f t="shared" ref="H3:H14" si="0">DATE(2025,3,2)</f>
+        <f t="shared" ref="H3:H7" si="0">DATE(2025,3,2)</f>
         <v>45718</v>
       </c>
     </row>
@@ -1804,7 +2281,7 @@
         <v>7</v>
       </c>
       <c r="H9" s="8">
-        <f t="shared" ref="H8:H19" si="1">DATE(2025,3,2)+14</f>
+        <f t="shared" ref="H9:H13" si="1">DATE(2025,3,2)+14</f>
         <v>45732</v>
       </c>
     </row>
@@ -1939,7 +2416,7 @@
         <v>7</v>
       </c>
       <c r="H14" s="8">
-        <f t="shared" ref="H14:H22" si="2">DATE(2025,3,2)+28</f>
+        <f t="shared" ref="H14:H16" si="2">DATE(2025,3,2)+28</f>
         <v>45746</v>
       </c>
     </row>
@@ -2290,7 +2767,7 @@
         <v>7</v>
       </c>
       <c r="H27" s="8">
-        <f t="shared" ref="H24:H31" si="4">DATE(2025,3,2)+42</f>
+        <f t="shared" ref="H27:H31" si="4">DATE(2025,3,2)+42</f>
         <v>45760</v>
       </c>
     </row>
@@ -2425,7 +2902,7 @@
         <v>7</v>
       </c>
       <c r="H32" s="8">
-        <f t="shared" ref="H26:H39" si="5">DATE(2025,3,2)+49</f>
+        <f t="shared" ref="H32:H39" si="5">DATE(2025,3,2)+49</f>
         <v>45767</v>
       </c>
     </row>
@@ -2641,7 +3118,7 @@
         <v>7</v>
       </c>
       <c r="H40" s="8">
-        <f t="shared" ref="H36:H41" si="6">DATE(2025,3,2)+56</f>
+        <f t="shared" ref="H40" si="6">DATE(2025,3,2)+56</f>
         <v>45774</v>
       </c>
     </row>
@@ -2695,7 +3172,7 @@
         <v>7</v>
       </c>
       <c r="H42" s="8">
-        <f t="shared" ref="H42:H49" si="7">DATE(2025,3,2)+56</f>
+        <f t="shared" ref="H42:H47" si="7">DATE(2025,3,2)+56</f>
         <v>45774</v>
       </c>
     </row>
@@ -2938,7 +3415,7 @@
         <v>7</v>
       </c>
       <c r="H51" s="8">
-        <f t="shared" ref="H50:H57" si="8">DATE(2025,3,2)+63</f>
+        <f t="shared" ref="H51:H56" si="8">DATE(2025,3,2)+63</f>
         <v>45781</v>
       </c>
     </row>
@@ -3113,7 +3590,7 @@
         <v>7</v>
       </c>
       <c r="H58" s="8">
-        <f t="shared" ref="H58:H71" si="9">DATE(2025,3,2)+70</f>
+        <f t="shared" ref="H58:H72" si="9">DATE(2025,3,2)+70</f>
         <v>45788</v>
       </c>
     </row>
@@ -3469,8 +3946,895 @@
       </c>
     </row>
     <row r="72" spans="1:8">
-      <c r="E72"/>
-      <c r="F72"/>
+      <c r="A72" s="4" t="s">
+        <v>381</v>
+      </c>
+      <c r="B72" t="s">
+        <v>53</v>
+      </c>
+      <c r="C72" t="s">
+        <v>328</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="E72" t="s">
+        <v>330</v>
+      </c>
+      <c r="F72" t="s">
+        <v>331</v>
+      </c>
+      <c r="G72" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H72" s="8">
+        <f>DATE(2025,3,2)+73</f>
+        <v>45791</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8">
+      <c r="A73" s="4" t="s">
+        <v>382</v>
+      </c>
+      <c r="B73" t="s">
+        <v>53</v>
+      </c>
+      <c r="C73" t="s">
+        <v>332</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="E73" t="s">
+        <v>334</v>
+      </c>
+      <c r="F73" t="s">
+        <v>335</v>
+      </c>
+      <c r="G73" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H73" s="8">
+        <f t="shared" ref="H73:H104" si="10">DATE(2025,3,2)+73</f>
+        <v>45791</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8">
+      <c r="A74" s="4" t="s">
+        <v>383</v>
+      </c>
+      <c r="B74" t="s">
+        <v>53</v>
+      </c>
+      <c r="C74" t="s">
+        <v>336</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="E74" t="s">
+        <v>338</v>
+      </c>
+      <c r="F74" t="s">
+        <v>339</v>
+      </c>
+      <c r="G74" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H74" s="8">
+        <f t="shared" si="10"/>
+        <v>45791</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8">
+      <c r="A75" s="4" t="s">
+        <v>384</v>
+      </c>
+      <c r="B75" t="s">
+        <v>53</v>
+      </c>
+      <c r="C75" t="s">
+        <v>340</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="E75" t="s">
+        <v>342</v>
+      </c>
+      <c r="F75" t="s">
+        <v>342</v>
+      </c>
+      <c r="G75" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H75" s="8">
+        <f t="shared" si="10"/>
+        <v>45791</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8">
+      <c r="A76" s="4" t="s">
+        <v>385</v>
+      </c>
+      <c r="B76" t="s">
+        <v>53</v>
+      </c>
+      <c r="C76" t="s">
+        <v>343</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="E76" t="s">
+        <v>345</v>
+      </c>
+      <c r="F76" t="s">
+        <v>346</v>
+      </c>
+      <c r="G76" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H76" s="8">
+        <f t="shared" si="10"/>
+        <v>45791</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8">
+      <c r="A77" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="B77" t="s">
+        <v>53</v>
+      </c>
+      <c r="C77" t="s">
+        <v>347</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="E77" t="s">
+        <v>345</v>
+      </c>
+      <c r="F77" t="s">
+        <v>346</v>
+      </c>
+      <c r="G77" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H77" s="8">
+        <f t="shared" si="10"/>
+        <v>45791</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8">
+      <c r="A78" s="4" t="s">
+        <v>387</v>
+      </c>
+      <c r="B78" t="s">
+        <v>53</v>
+      </c>
+      <c r="C78" t="s">
+        <v>349</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="E78" t="s">
+        <v>351</v>
+      </c>
+      <c r="F78" t="s">
+        <v>352</v>
+      </c>
+      <c r="G78" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H78" s="8">
+        <f t="shared" si="10"/>
+        <v>45791</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8">
+      <c r="A79" s="4" t="s">
+        <v>388</v>
+      </c>
+      <c r="B79" t="s">
+        <v>53</v>
+      </c>
+      <c r="C79" t="s">
+        <v>353</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="E79" t="s">
+        <v>355</v>
+      </c>
+      <c r="F79" t="s">
+        <v>355</v>
+      </c>
+      <c r="G79" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H79" s="8">
+        <f t="shared" si="10"/>
+        <v>45791</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8">
+      <c r="A80" s="4" t="s">
+        <v>389</v>
+      </c>
+      <c r="B80" t="s">
+        <v>104</v>
+      </c>
+      <c r="C80" t="s">
+        <v>356</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="E80" t="s">
+        <v>358</v>
+      </c>
+      <c r="F80" t="s">
+        <v>359</v>
+      </c>
+      <c r="G80" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H80" s="8">
+        <f t="shared" si="10"/>
+        <v>45791</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8">
+      <c r="A81" s="4" t="s">
+        <v>390</v>
+      </c>
+      <c r="B81" t="s">
+        <v>104</v>
+      </c>
+      <c r="C81" t="s">
+        <v>360</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="E81" t="s">
+        <v>362</v>
+      </c>
+      <c r="F81" t="s">
+        <v>363</v>
+      </c>
+      <c r="G81" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H81" s="8">
+        <f t="shared" si="10"/>
+        <v>45791</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8">
+      <c r="A82" s="4" t="s">
+        <v>391</v>
+      </c>
+      <c r="B82" t="s">
+        <v>104</v>
+      </c>
+      <c r="C82" t="s">
+        <v>364</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="E82" t="s">
+        <v>171</v>
+      </c>
+      <c r="F82" t="s">
+        <v>363</v>
+      </c>
+      <c r="G82" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H82" s="8">
+        <f t="shared" si="10"/>
+        <v>45791</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8">
+      <c r="A83" s="4" t="s">
+        <v>392</v>
+      </c>
+      <c r="B83" t="s">
+        <v>53</v>
+      </c>
+      <c r="C83" t="s">
+        <v>366</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="E83" t="s">
+        <v>368</v>
+      </c>
+      <c r="F83" t="s">
+        <v>369</v>
+      </c>
+      <c r="G83" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H83" s="8">
+        <f t="shared" si="10"/>
+        <v>45791</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8">
+      <c r="A84" s="4" t="s">
+        <v>393</v>
+      </c>
+      <c r="B84" t="s">
+        <v>53</v>
+      </c>
+      <c r="C84" t="s">
+        <v>370</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="E84" t="s">
+        <v>372</v>
+      </c>
+      <c r="F84" t="s">
+        <v>363</v>
+      </c>
+      <c r="G84" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H84" s="8">
+        <f t="shared" si="10"/>
+        <v>45791</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8">
+      <c r="A85" s="4" t="s">
+        <v>394</v>
+      </c>
+      <c r="B85" t="s">
+        <v>53</v>
+      </c>
+      <c r="C85" t="s">
+        <v>373</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="E85" t="s">
+        <v>375</v>
+      </c>
+      <c r="F85" t="s">
+        <v>376</v>
+      </c>
+      <c r="G85" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H85" s="8">
+        <f t="shared" si="10"/>
+        <v>45791</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8">
+      <c r="A86" s="4" t="s">
+        <v>395</v>
+      </c>
+      <c r="B86" t="s">
+        <v>53</v>
+      </c>
+      <c r="C86" t="s">
+        <v>377</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="E86" t="s">
+        <v>379</v>
+      </c>
+      <c r="F86" t="s">
+        <v>380</v>
+      </c>
+      <c r="G86" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H86" s="8">
+        <f t="shared" si="10"/>
+        <v>45791</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" s="1" customFormat="1" ht="30">
+      <c r="A87" s="4" t="s">
+        <v>469</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="F87" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="G87" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H87" s="8">
+        <f t="shared" si="10"/>
+        <v>45791</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" s="1" customFormat="1">
+      <c r="A88" s="4" t="s">
+        <v>470</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="F88" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="G88" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H88" s="8">
+        <f t="shared" si="10"/>
+        <v>45791</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" s="1" customFormat="1">
+      <c r="A89" s="4" t="s">
+        <v>471</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="F89" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="G89" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H89" s="8">
+        <f t="shared" si="10"/>
+        <v>45791</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" s="1" customFormat="1" ht="30">
+      <c r="A90" s="4" t="s">
+        <v>472</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="F90" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="G90" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H90" s="8">
+        <f t="shared" si="10"/>
+        <v>45791</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" s="1" customFormat="1" ht="30">
+      <c r="A91" s="4" t="s">
+        <v>473</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="F91" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="G91" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H91" s="8">
+        <f t="shared" si="10"/>
+        <v>45791</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" s="1" customFormat="1" ht="30">
+      <c r="A92" s="4" t="s">
+        <v>474</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="F92" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="G92" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H92" s="8">
+        <f t="shared" si="10"/>
+        <v>45791</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" s="1" customFormat="1" ht="30">
+      <c r="A93" s="4" t="s">
+        <v>475</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="F93" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="G93" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H93" s="8">
+        <f t="shared" si="10"/>
+        <v>45791</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" s="1" customFormat="1">
+      <c r="A94" s="4" t="s">
+        <v>476</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="F94" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="G94" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H94" s="8">
+        <f t="shared" si="10"/>
+        <v>45791</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" s="1" customFormat="1">
+      <c r="A95" s="4" t="s">
+        <v>477</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="F95" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="G95" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H95" s="8">
+        <f t="shared" si="10"/>
+        <v>45791</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" s="1" customFormat="1">
+      <c r="A96" s="4" t="s">
+        <v>478</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="F96" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="G96" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H96" s="8">
+        <f t="shared" si="10"/>
+        <v>45791</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" s="1" customFormat="1">
+      <c r="A97" s="4" t="s">
+        <v>479</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="E97" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="F97" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="G97" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H97" s="8">
+        <f t="shared" si="10"/>
+        <v>45791</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" s="1" customFormat="1" ht="30">
+      <c r="A98" s="4" t="s">
+        <v>480</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="E98" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="F98" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="G98" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H98" s="8">
+        <f t="shared" si="10"/>
+        <v>45791</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" s="1" customFormat="1">
+      <c r="A99" s="4" t="s">
+        <v>481</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="E99" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="F99" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="G99" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H99" s="8">
+        <f t="shared" si="10"/>
+        <v>45791</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" s="1" customFormat="1">
+      <c r="A100" s="4" t="s">
+        <v>482</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="D100" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="E100" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="F100" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="G100" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H100" s="8">
+        <f t="shared" si="10"/>
+        <v>45791</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" s="1" customFormat="1">
+      <c r="A101" s="4" t="s">
+        <v>483</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="E101" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="F101" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="G101" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H101" s="8">
+        <f t="shared" si="10"/>
+        <v>45791</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" s="1" customFormat="1">
+      <c r="A102" s="4" t="s">
+        <v>484</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="E102" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="F102" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="G102" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H102" s="8">
+        <f t="shared" si="10"/>
+        <v>45791</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" s="1" customFormat="1">
+      <c r="A103" s="4" t="s">
+        <v>485</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="E103" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="F103" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="G103" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H103" s="8">
+        <f t="shared" si="10"/>
+        <v>45791</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" s="1" customFormat="1">
+      <c r="A104" s="4" t="s">
+        <v>486</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="E104" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="F104" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="G104" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H104" s="8">
+        <f t="shared" si="10"/>
+        <v>45791</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>